<commit_message>
cleaning from intermediate results
Rimozione di variabili create per vedere valori intermedi mentre il modello veniva creato
</commit_message>
<xml_diff>
--- a/thesis/main/sets.xlsx
+++ b/thesis/main/sets.xlsx
@@ -8,26 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_tesi/thesis/main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B18C5AB-76D4-C14E-96C7-562022AE1589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE15B70-3B99-6646-BC79-039567F64484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_set_days" sheetId="1" r:id="rId1"/>
     <sheet name="_set_th" sheetId="2" r:id="rId2"/>
-    <sheet name="_set_th2" sheetId="3" r:id="rId3"/>
-    <sheet name="_set_needs" sheetId="4" r:id="rId4"/>
-    <sheet name="_set_f" sheetId="5" r:id="rId5"/>
-    <sheet name="_set_t" sheetId="6" r:id="rId6"/>
-    <sheet name="_set_a" sheetId="7" r:id="rId7"/>
-    <sheet name="_set_s" sheetId="8" r:id="rId8"/>
+    <sheet name="_set_needs" sheetId="4" r:id="rId3"/>
+    <sheet name="_set_f" sheetId="5" r:id="rId4"/>
+    <sheet name="_set_t" sheetId="6" r:id="rId5"/>
+    <sheet name="_set_a" sheetId="7" r:id="rId6"/>
+    <sheet name="_set_s" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="98">
   <si>
     <t>days_names</t>
   </si>
@@ -39,9 +38,6 @@
   </si>
   <si>
     <t>days</t>
-  </si>
-  <si>
-    <t>th2_names</t>
   </si>
   <si>
     <t>n_names</t>
@@ -718,17 +714,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -759,68 +755,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -828,10 +824,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -840,11 +836,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -854,34 +850,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
+    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -890,81 +911,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -976,186 +922,186 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1163,7 +1109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
@@ -1175,211 +1121,211 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1387,7 +1333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -1399,255 +1345,255 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1655,11 +1601,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -1667,12 +1613,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>